<commit_message>
Add example .csv files
</commit_message>
<xml_diff>
--- a/inst/example_input_xlsx/demo_admat_input.xlsx
+++ b/inst/example_input_xlsx/demo_admat_input.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C20093-9A6B-455E-B1A7-7AE7F90DB18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D3CDD2-8232-4896-9EA7-32B8C4EBB364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4815" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summer" sheetId="1" r:id="rId1"/>
@@ -428,27 +428,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="A1:G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1"/>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1"/>
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -456,7 +461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -467,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -478,7 +483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -494,27 +499,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="A1:H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1"/>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -522,7 +533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -533,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -544,7 +555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -560,27 +571,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1"/>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -591,7 +606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -602,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -613,7 +628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -629,27 +644,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="A1:F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1"/>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -657,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -668,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -679,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updates to demo data
</commit_message>
<xml_diff>
--- a/inst/example_input_xlsx/demo_admat_input.xlsx
+++ b/inst/example_input_xlsx/demo_admat_input.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D3CDD2-8232-4896-9EA7-32B8C4EBB364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF20FE6-558A-4A2C-A38D-601BBDC4D4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4815" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4815" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summer" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="7">
   <si>
     <t>Det</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>0.01, 0.6</t>
-  </si>
-  <si>
-    <t>0.1</t>
   </si>
   <si>
     <t>0.6</t>
@@ -430,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
@@ -573,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,9 +599,6 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -614,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -625,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>